<commit_message>
updated templates and code
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Kogel-Knabner_2008_SvF.xlsx
+++ b/ISRaD_data_files/Kogel-Knabner_2008_SvF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20387"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfromm\Documents\GitHub\ISRaD_SvF\ISRaD_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6429901A-3B4A-440E-A60D-511148A7B05D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDF1BAD-62F3-4C14-ADF5-0AC6D26CD5A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25164" windowHeight="14580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25164" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="incubation" sheetId="8" r:id="rId8"/>
     <sheet name="controlled vocabulary" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="942">
   <si>
     <t>entry_name</t>
   </si>
@@ -1389,12 +1389,6 @@
     <t>Ah</t>
   </si>
   <si>
-    <t>43.6</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Steinkreuz2:49.872,10.461_338_0_5</t>
   </si>
   <si>
@@ -1404,9 +1398,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>82.6</t>
-  </si>
-  <si>
     <t>Steinkreuz:49.872,10.461_248_5_24</t>
   </si>
   <si>
@@ -1416,9 +1407,6 @@
     <t>Bv</t>
   </si>
   <si>
-    <t>24.5</t>
-  </si>
-  <si>
     <t>Waldstein2:50.1,11.85_339_10_12</t>
   </si>
   <si>
@@ -1431,42 +1419,27 @@
     <t>Bh</t>
   </si>
   <si>
-    <t>92.8</t>
-  </si>
-  <si>
     <t>Waldstein2:50.1,11.85_339_0_10</t>
   </si>
   <si>
     <t>EA</t>
   </si>
   <si>
-    <t>38.1</t>
-  </si>
-  <si>
     <t>Steinkreuz2:49.872,10.461_338_5_24</t>
   </si>
   <si>
     <t>Bw1</t>
   </si>
   <si>
-    <t>9.8</t>
-  </si>
-  <si>
     <t>Waldstein:50.1,11.85_247_10_12</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Waldstein:50.1,11.85_247_0_10</t>
   </si>
   <si>
     <t>Aeh</t>
   </si>
   <si>
-    <t>16.6</t>
-  </si>
-  <si>
     <t>Waldstein2:50.1,11.85_339_12_30</t>
   </si>
   <si>
@@ -1476,9 +1449,6 @@
     <t>Bs</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>Steinkreuz:49.872,10.461_248_24_50</t>
   </si>
   <si>
@@ -1488,18 +1458,12 @@
     <t>SwBv1</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>Waldstein:50.1,11.85_247_12_30</t>
   </si>
   <si>
     <t>Bvs</t>
   </si>
   <si>
-    <t>31.4</t>
-  </si>
-  <si>
     <t>Steinkreuz2:49.872,10.461_338_24_50</t>
   </si>
   <si>
@@ -1521,9 +1485,6 @@
     <t>Bw</t>
   </si>
   <si>
-    <t>7.7</t>
-  </si>
-  <si>
     <t>Steinkreuz:49.872,10.461_248_50_80</t>
   </si>
   <si>
@@ -1533,9 +1494,6 @@
     <t>SwBv2</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Steinkreuz:49.872,10.461_248_85_115</t>
   </si>
   <si>
@@ -1548,9 +1506,6 @@
     <t>IIICv</t>
   </si>
   <si>
-    <t>1.3</t>
-  </si>
-  <si>
     <t>Steinkreuz:49.872,10.461_248_115_140</t>
   </si>
   <si>
@@ -1560,36 +1515,24 @@
     <t>IVCv</t>
   </si>
   <si>
-    <t>0.7</t>
-  </si>
-  <si>
     <t>Steinkreuz2:49.872,10.461_338_85_115</t>
   </si>
   <si>
     <t>3C</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>Steinkreuz2:49.872,10.461_338_50_80</t>
   </si>
   <si>
     <t>Bw3</t>
   </si>
   <si>
-    <t>1.4</t>
-  </si>
-  <si>
     <t>Steinkreuz2:49.872,10.461_338_115_140</t>
   </si>
   <si>
     <t>4C1</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>Waldstein:50.1,11.85_247_70_80</t>
   </si>
   <si>
@@ -1599,25 +1542,16 @@
     <t>Cv2</t>
   </si>
   <si>
-    <t>1.2</t>
-  </si>
-  <si>
     <t>Waldstein2:50.1,11.85_339_55_70</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>1.7</t>
-  </si>
-  <si>
     <t>Waldstein2:50.1,11.85_339_70_80</t>
   </si>
   <si>
     <t>C2</t>
-  </si>
-  <si>
-    <t>1.9</t>
   </si>
   <si>
     <t>Waldstein:50.1,11.85_337_70_80</t>
@@ -3046,9 +2980,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3350,7 +3282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -3491,7 +3423,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3624,7 +3556,7 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C4" t="s">
         <v>70</v>
@@ -3641,7 +3573,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C5" t="s">
         <v>73</v>
@@ -3668,7 +3600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4:N8"/>
     </sheetView>
   </sheetViews>
@@ -3718,7 +3650,7 @@
         <v>86</v>
       </c>
       <c r="N1" t="s">
-        <v>963</v>
+        <v>941</v>
       </c>
       <c r="O1" t="s">
         <v>87</v>
@@ -4000,7 +3932,7 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="D4" t="s">
         <v>163</v>
@@ -4020,7 +3952,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="D5" t="s">
         <v>168</v>
@@ -4040,7 +3972,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="D6" t="s">
         <v>169</v>
@@ -4060,7 +3992,7 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="D7" t="s">
         <v>171</v>
@@ -4080,7 +4012,7 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="D8" t="s">
         <v>172</v>
@@ -4433,7 +4365,7 @@
   <dimension ref="A1:CT27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BC4" sqref="BC4:BD27"/>
+      <selection activeCell="AO4" sqref="AO4:AP27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5277,7 +5209,7 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C4" t="s">
         <v>163</v>
@@ -5297,8 +5229,8 @@
       <c r="K4" t="s">
         <v>450</v>
       </c>
-      <c r="AO4" t="s">
-        <v>451</v>
+      <c r="AN4">
+        <v>4.3600000000000003</v>
       </c>
       <c r="BC4" s="1">
         <v>1.123</v>
@@ -5312,13 +5244,13 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C5" t="s">
         <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E5" t="s">
         <v>447</v>
@@ -5327,13 +5259,13 @@
         <v>449</v>
       </c>
       <c r="J5" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="K5" t="s">
-        <v>459</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>460</v>
+        <v>456</v>
+      </c>
+      <c r="AN5">
+        <v>2.4500000000000002</v>
       </c>
       <c r="BC5" s="1">
         <v>1.0129999999999999</v>
@@ -5347,28 +5279,28 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C6" t="s">
         <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="E6" t="s">
         <v>447</v>
       </c>
       <c r="I6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J6" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="K6" t="s">
-        <v>483</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>484</v>
+        <v>473</v>
+      </c>
+      <c r="AN6">
+        <v>0.8</v>
       </c>
       <c r="BC6" s="1">
         <v>0.92099999999999993</v>
@@ -5382,28 +5314,28 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C7" t="s">
         <v>163</v>
       </c>
       <c r="D7" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="E7" t="s">
         <v>447</v>
       </c>
       <c r="I7" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="J7" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="K7" t="s">
-        <v>498</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>499</v>
+        <v>485</v>
+      </c>
+      <c r="AN7">
+        <v>0.4</v>
       </c>
       <c r="BC7" s="1">
         <v>0.80900000000000005</v>
@@ -5417,28 +5349,28 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C8" t="s">
         <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="E8" t="s">
         <v>447</v>
       </c>
       <c r="I8" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="J8" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="K8" t="s">
-        <v>503</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>504</v>
+        <v>489</v>
+      </c>
+      <c r="AN8">
+        <v>0.13</v>
       </c>
       <c r="BC8" s="1">
         <v>0.80599999999999994</v>
@@ -5452,28 +5384,28 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C9" t="s">
         <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="E9" t="s">
         <v>447</v>
       </c>
       <c r="I9" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="J9" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
       <c r="K9" t="s">
-        <v>507</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>508</v>
+        <v>492</v>
+      </c>
+      <c r="AN9">
+        <v>6.9999999999999993E-2</v>
       </c>
       <c r="BC9" s="1">
         <v>0.76300000000000001</v>
@@ -5487,16 +5419,16 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C10" t="s">
         <v>168</v>
       </c>
       <c r="D10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I10" t="s">
         <v>448</v>
@@ -5505,10 +5437,10 @@
         <v>449</v>
       </c>
       <c r="K10" t="s">
-        <v>455</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>456</v>
+        <v>453</v>
+      </c>
+      <c r="AN10">
+        <v>8.26</v>
       </c>
       <c r="BC10" s="1">
         <v>1.119</v>
@@ -5522,28 +5454,28 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C11" t="s">
         <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I11" t="s">
         <v>449</v>
       </c>
       <c r="J11" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="K11" t="s">
-        <v>470</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>471</v>
+        <v>464</v>
+      </c>
+      <c r="AN11">
+        <v>0.98000000000000009</v>
       </c>
       <c r="BC11" s="1">
         <v>0.98</v>
@@ -5557,28 +5489,28 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C12" t="s">
         <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="E12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I12" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J12" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="K12" t="s">
-        <v>489</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>452</v>
+        <v>477</v>
+      </c>
+      <c r="AN12">
+        <v>0.3</v>
       </c>
       <c r="BC12" s="1">
         <v>0.84200000000000008</v>
@@ -5592,28 +5524,28 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C13" t="s">
         <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="E13" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I13" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="J13" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="K13" t="s">
-        <v>510</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>511</v>
+        <v>494</v>
+      </c>
+      <c r="AN13">
+        <v>0.11000000000000001</v>
       </c>
       <c r="BC13" s="1">
         <v>0.70799999999999996</v>
@@ -5627,28 +5559,28 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C14" t="s">
         <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
       <c r="E14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I14" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="J14" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="K14" t="s">
-        <v>513</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>514</v>
+        <v>496</v>
+      </c>
+      <c r="AN14">
+        <v>0.13999999999999999</v>
       </c>
       <c r="BC14" s="1">
         <v>0.69799999999999995</v>
@@ -5662,28 +5594,28 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>958</v>
+        <v>936</v>
       </c>
       <c r="C15" t="s">
         <v>168</v>
       </c>
       <c r="D15" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
       <c r="E15" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I15" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="J15" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
       <c r="K15" t="s">
-        <v>516</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>517</v>
+        <v>498</v>
+      </c>
+      <c r="AN15">
+        <v>0.05</v>
       </c>
       <c r="BC15" s="1">
         <v>0.69099999999999995</v>
@@ -5697,28 +5629,28 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C16" t="s">
         <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="E16" t="s">
         <v>447</v>
       </c>
       <c r="I16" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="J16" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="K16" t="s">
-        <v>464</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>473</v>
+        <v>460</v>
+      </c>
+      <c r="AN16">
+        <v>0.6</v>
       </c>
       <c r="BC16" s="1">
         <v>0.98499999999999999</v>
@@ -5732,13 +5664,13 @@
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C17" t="s">
         <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="E17" t="s">
         <v>447</v>
@@ -5747,13 +5679,13 @@
         <v>448</v>
       </c>
       <c r="J17" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="K17" t="s">
-        <v>475</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>476</v>
+        <v>467</v>
+      </c>
+      <c r="AN17">
+        <v>1.6600000000000001</v>
       </c>
       <c r="BC17" s="1">
         <v>0.93599999999999994</v>
@@ -5767,28 +5699,28 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C18" t="s">
         <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="E18" t="s">
         <v>447</v>
       </c>
       <c r="I18" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="J18" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="K18" t="s">
-        <v>486</v>
-      </c>
-      <c r="AO18" t="s">
-        <v>487</v>
+        <v>475</v>
+      </c>
+      <c r="AN18">
+        <v>3.1399999999999997</v>
       </c>
       <c r="BC18" s="1">
         <v>0.91099999999999992</v>
@@ -5802,28 +5734,28 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C19" t="s">
         <v>171</v>
       </c>
       <c r="D19" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="E19" t="s">
         <v>447</v>
       </c>
       <c r="I19" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="J19" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="K19" t="s">
-        <v>492</v>
-      </c>
-      <c r="AO19" t="s">
-        <v>463</v>
+        <v>480</v>
+      </c>
+      <c r="AN19">
+        <v>1.2</v>
       </c>
       <c r="BC19" s="1">
         <v>0.82200000000000006</v>
@@ -5837,28 +5769,28 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C20" t="s">
         <v>171</v>
       </c>
       <c r="D20" t="s">
-        <v>518</v>
+        <v>499</v>
       </c>
       <c r="E20" t="s">
         <v>447</v>
       </c>
       <c r="I20" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="J20" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="K20" t="s">
-        <v>520</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>521</v>
+        <v>501</v>
+      </c>
+      <c r="AN20">
+        <v>0.12</v>
       </c>
       <c r="BC20" s="1">
         <v>0.62</v>
@@ -5872,28 +5804,28 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C21" t="s">
         <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>528</v>
+        <v>506</v>
       </c>
       <c r="E21" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I21" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="J21" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="K21" t="s">
-        <v>526</v>
-      </c>
-      <c r="AO21" t="s">
-        <v>527</v>
+        <v>505</v>
+      </c>
+      <c r="AN21">
+        <v>0.19</v>
       </c>
       <c r="BC21" s="1">
         <v>0.52</v>
@@ -5907,28 +5839,28 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C22" t="s">
         <v>169</v>
       </c>
       <c r="D22" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E22" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I22" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="J22" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="K22" t="s">
-        <v>464</v>
-      </c>
-      <c r="AO22" t="s">
-        <v>465</v>
+        <v>460</v>
+      </c>
+      <c r="AN22">
+        <v>9.2799999999999994</v>
       </c>
       <c r="BC22" s="1">
         <v>0.995</v>
@@ -5942,28 +5874,28 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C23" t="s">
         <v>169</v>
       </c>
       <c r="D23" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I23" t="s">
         <v>448</v>
       </c>
       <c r="J23" t="s">
+        <v>458</v>
+      </c>
+      <c r="K23" t="s">
         <v>462</v>
       </c>
-      <c r="K23" t="s">
-        <v>467</v>
-      </c>
-      <c r="AO23" t="s">
-        <v>468</v>
+      <c r="AN23">
+        <v>3.81</v>
       </c>
       <c r="BC23" s="1">
         <v>0.98499999999999999</v>
@@ -5977,28 +5909,28 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C24" t="s">
         <v>169</v>
       </c>
       <c r="D24" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="E24" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I24" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="J24" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="K24" t="s">
-        <v>479</v>
-      </c>
-      <c r="AO24" t="s">
-        <v>480</v>
+        <v>470</v>
+      </c>
+      <c r="AN24">
+        <v>5.2</v>
       </c>
       <c r="BC24" s="1">
         <v>0.92200000000000004</v>
@@ -6012,28 +5944,28 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C25" t="s">
         <v>169</v>
       </c>
       <c r="D25" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="E25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I25" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="J25" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="K25" t="s">
-        <v>494</v>
-      </c>
-      <c r="AO25" t="s">
-        <v>495</v>
+        <v>482</v>
+      </c>
+      <c r="AN25">
+        <v>0.77</v>
       </c>
       <c r="BC25" s="1">
         <v>0.81499999999999995</v>
@@ -6047,28 +5979,28 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C26" t="s">
         <v>169</v>
       </c>
       <c r="D26" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
       <c r="E26" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I26" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="J26" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="K26" t="s">
-        <v>523</v>
-      </c>
-      <c r="AO26" t="s">
-        <v>524</v>
+        <v>503</v>
+      </c>
+      <c r="AN26">
+        <v>0.16999999999999998</v>
       </c>
       <c r="BC26" s="1">
         <v>0.58799999999999997</v>
@@ -6082,28 +6014,28 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>959</v>
+        <v>937</v>
       </c>
       <c r="C27" t="s">
         <v>169</v>
       </c>
       <c r="D27" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="E27" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I27" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="J27" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="K27" t="s">
-        <v>526</v>
-      </c>
-      <c r="AO27" t="s">
-        <v>527</v>
+        <v>505</v>
+      </c>
+      <c r="AN27">
+        <v>0.19</v>
       </c>
       <c r="BC27" s="1">
         <v>0.56499999999999995</v>
@@ -6145,79 +6077,79 @@
         <v>77</v>
       </c>
       <c r="D1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E1" t="s">
+        <v>508</v>
+      </c>
+      <c r="F1" t="s">
+        <v>509</v>
+      </c>
+      <c r="G1" t="s">
+        <v>510</v>
+      </c>
+      <c r="H1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I1" t="s">
+        <v>512</v>
+      </c>
+      <c r="J1" t="s">
+        <v>513</v>
+      </c>
+      <c r="K1" t="s">
+        <v>514</v>
+      </c>
+      <c r="L1" t="s">
+        <v>515</v>
+      </c>
+      <c r="M1" t="s">
+        <v>516</v>
+      </c>
+      <c r="N1" t="s">
+        <v>517</v>
+      </c>
+      <c r="O1" t="s">
+        <v>518</v>
+      </c>
+      <c r="P1" t="s">
+        <v>519</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>520</v>
+      </c>
+      <c r="R1" t="s">
+        <v>521</v>
+      </c>
+      <c r="S1" t="s">
+        <v>522</v>
+      </c>
+      <c r="T1" t="s">
+        <v>523</v>
+      </c>
+      <c r="U1" t="s">
+        <v>524</v>
+      </c>
+      <c r="V1" t="s">
+        <v>525</v>
+      </c>
+      <c r="W1" t="s">
+        <v>526</v>
+      </c>
+      <c r="X1" t="s">
+        <v>527</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z1" t="s">
         <v>529</v>
       </c>
-      <c r="E1" t="s">
+      <c r="AA1" t="s">
         <v>530</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AB1" t="s">
         <v>531</v>
-      </c>
-      <c r="G1" t="s">
-        <v>532</v>
-      </c>
-      <c r="H1" t="s">
-        <v>533</v>
-      </c>
-      <c r="I1" t="s">
-        <v>534</v>
-      </c>
-      <c r="J1" t="s">
-        <v>535</v>
-      </c>
-      <c r="K1" t="s">
-        <v>536</v>
-      </c>
-      <c r="L1" t="s">
-        <v>537</v>
-      </c>
-      <c r="M1" t="s">
-        <v>538</v>
-      </c>
-      <c r="N1" t="s">
-        <v>539</v>
-      </c>
-      <c r="O1" t="s">
-        <v>540</v>
-      </c>
-      <c r="P1" t="s">
-        <v>541</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>542</v>
-      </c>
-      <c r="R1" t="s">
-        <v>543</v>
-      </c>
-      <c r="S1" t="s">
-        <v>544</v>
-      </c>
-      <c r="T1" t="s">
-        <v>545</v>
-      </c>
-      <c r="U1" t="s">
-        <v>546</v>
-      </c>
-      <c r="V1" t="s">
-        <v>547</v>
-      </c>
-      <c r="W1" t="s">
-        <v>548</v>
-      </c>
-      <c r="X1" t="s">
-        <v>549</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>550</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>551</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>552</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -6240,25 +6172,25 @@
         <v>211</v>
       </c>
       <c r="G2" t="s">
-        <v>554</v>
+        <v>532</v>
       </c>
       <c r="H2" t="s">
-        <v>555</v>
+        <v>533</v>
       </c>
       <c r="I2" t="s">
-        <v>556</v>
+        <v>534</v>
       </c>
       <c r="J2" t="s">
-        <v>557</v>
+        <v>535</v>
       </c>
       <c r="K2" t="s">
-        <v>558</v>
+        <v>536</v>
       </c>
       <c r="L2" t="s">
-        <v>559</v>
+        <v>537</v>
       </c>
       <c r="M2" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="N2" t="s">
         <v>223</v>
@@ -6267,13 +6199,13 @@
         <v>224</v>
       </c>
       <c r="P2" t="s">
-        <v>561</v>
+        <v>539</v>
       </c>
       <c r="R2" t="s">
-        <v>562</v>
+        <v>540</v>
       </c>
       <c r="S2" t="s">
-        <v>563</v>
+        <v>541</v>
       </c>
       <c r="T2" t="s">
         <v>230</v>
@@ -6285,22 +6217,22 @@
         <v>232</v>
       </c>
       <c r="W2" t="s">
-        <v>564</v>
+        <v>542</v>
       </c>
       <c r="X2" t="s">
-        <v>565</v>
+        <v>543</v>
       </c>
       <c r="Y2" t="s">
-        <v>566</v>
+        <v>544</v>
       </c>
       <c r="Z2" t="s">
-        <v>567</v>
+        <v>545</v>
       </c>
       <c r="AA2" t="s">
-        <v>568</v>
+        <v>546</v>
       </c>
       <c r="AB2" t="s">
-        <v>569</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
@@ -6320,10 +6252,10 @@
         <v>153</v>
       </c>
       <c r="H3" t="s">
-        <v>570</v>
+        <v>548</v>
       </c>
       <c r="L3" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="M3" t="s">
         <v>246</v>
@@ -6385,211 +6317,211 @@
         <v>251</v>
       </c>
       <c r="E1" t="s">
+        <v>550</v>
+      </c>
+      <c r="F1" t="s">
+        <v>551</v>
+      </c>
+      <c r="G1" t="s">
+        <v>552</v>
+      </c>
+      <c r="H1" t="s">
+        <v>553</v>
+      </c>
+      <c r="I1" t="s">
+        <v>554</v>
+      </c>
+      <c r="J1" t="s">
+        <v>555</v>
+      </c>
+      <c r="K1" t="s">
+        <v>556</v>
+      </c>
+      <c r="L1" t="s">
+        <v>557</v>
+      </c>
+      <c r="M1" t="s">
+        <v>558</v>
+      </c>
+      <c r="N1" t="s">
+        <v>559</v>
+      </c>
+      <c r="O1" t="s">
+        <v>560</v>
+      </c>
+      <c r="P1" t="s">
+        <v>561</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>562</v>
+      </c>
+      <c r="R1" t="s">
+        <v>563</v>
+      </c>
+      <c r="S1" t="s">
+        <v>564</v>
+      </c>
+      <c r="T1" t="s">
+        <v>565</v>
+      </c>
+      <c r="U1" t="s">
+        <v>566</v>
+      </c>
+      <c r="V1" t="s">
+        <v>567</v>
+      </c>
+      <c r="W1" t="s">
+        <v>568</v>
+      </c>
+      <c r="X1" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>570</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>571</v>
+      </c>
+      <c r="AA1" t="s">
         <v>572</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AB1" t="s">
         <v>573</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AC1" t="s">
         <v>574</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AD1" t="s">
         <v>575</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AE1" t="s">
         <v>576</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AF1" t="s">
         <v>577</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AG1" t="s">
         <v>578</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AH1" t="s">
         <v>579</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="AL1" t="s">
         <v>580</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AM1" t="s">
         <v>581</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AN1" t="s">
         <v>582</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AO1" t="s">
         <v>583</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AP1" t="s">
         <v>584</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AQ1" t="s">
         <v>585</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AR1" t="s">
         <v>586</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AS1" t="s">
         <v>587</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AT1" t="s">
         <v>588</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AU1" t="s">
         <v>589</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AV1" t="s">
         <v>590</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AW1" t="s">
         <v>591</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AX1" t="s">
         <v>592</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AY1" t="s">
         <v>593</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AZ1" t="s">
         <v>594</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="BA1" t="s">
         <v>595</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="BB1" t="s">
         <v>596</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="BC1" t="s">
         <v>597</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="BD1" t="s">
         <v>598</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="BE1" t="s">
         <v>599</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="BF1" t="s">
         <v>600</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="BG1" t="s">
         <v>601</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>960</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>961</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>962</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="BH1" t="s">
         <v>602</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BI1" t="s">
         <v>603</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BJ1" t="s">
         <v>604</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BK1" t="s">
         <v>605</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BL1" t="s">
         <v>606</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BM1" t="s">
         <v>607</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BN1" t="s">
         <v>608</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BO1" t="s">
         <v>609</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BP1" t="s">
         <v>610</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BQ1" t="s">
         <v>611</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BR1" t="s">
         <v>612</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BS1" t="s">
         <v>613</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BT1" t="s">
         <v>614</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BU1" t="s">
         <v>615</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>616</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>617</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>618</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>619</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>620</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>621</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>622</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>623</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>624</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>625</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>626</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>627</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>628</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>629</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>630</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>631</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>632</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>633</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>634</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>635</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>636</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="2" spans="1:73" x14ac:dyDescent="0.3">
@@ -6606,40 +6538,40 @@
         <v>346</v>
       </c>
       <c r="E2" t="s">
-        <v>638</v>
+        <v>616</v>
       </c>
       <c r="F2" t="s">
-        <v>639</v>
+        <v>617</v>
       </c>
       <c r="G2" t="s">
-        <v>640</v>
+        <v>618</v>
       </c>
       <c r="H2" t="s">
-        <v>641</v>
+        <v>619</v>
       </c>
       <c r="I2" t="s">
-        <v>642</v>
+        <v>620</v>
       </c>
       <c r="J2" t="s">
-        <v>643</v>
+        <v>621</v>
       </c>
       <c r="K2" t="s">
-        <v>644</v>
+        <v>622</v>
       </c>
       <c r="L2" t="s">
-        <v>645</v>
+        <v>623</v>
       </c>
       <c r="M2" t="s">
-        <v>646</v>
+        <v>624</v>
       </c>
       <c r="N2" t="s">
-        <v>647</v>
+        <v>625</v>
       </c>
       <c r="O2" t="s">
-        <v>648</v>
+        <v>626</v>
       </c>
       <c r="P2" t="s">
-        <v>649</v>
+        <v>627</v>
       </c>
       <c r="Q2" t="s">
         <v>209</v>
@@ -6651,28 +6583,28 @@
         <v>211</v>
       </c>
       <c r="U2" t="s">
-        <v>650</v>
+        <v>628</v>
       </c>
       <c r="V2" t="s">
-        <v>651</v>
+        <v>629</v>
       </c>
       <c r="W2" t="s">
-        <v>652</v>
+        <v>630</v>
       </c>
       <c r="X2" t="s">
-        <v>653</v>
+        <v>631</v>
       </c>
       <c r="Y2" t="s">
-        <v>654</v>
+        <v>632</v>
       </c>
       <c r="Z2" t="s">
-        <v>655</v>
+        <v>633</v>
       </c>
       <c r="AA2" t="s">
-        <v>656</v>
+        <v>634</v>
       </c>
       <c r="AB2" t="s">
-        <v>657</v>
+        <v>635</v>
       </c>
       <c r="AC2" t="s">
         <v>230</v>
@@ -6684,22 +6616,22 @@
         <v>232</v>
       </c>
       <c r="AF2" t="s">
-        <v>658</v>
+        <v>636</v>
       </c>
       <c r="AG2" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
       <c r="AH2" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
       <c r="AI2" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
       <c r="AJ2" t="s">
-        <v>662</v>
+        <v>640</v>
       </c>
       <c r="AK2" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="AL2" t="s">
         <v>394</v>
@@ -6723,7 +6655,7 @@
         <v>403</v>
       </c>
       <c r="AS2" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
       <c r="AT2" t="s">
         <v>405</v>
@@ -6774,7 +6706,7 @@
         <v>421</v>
       </c>
       <c r="BJ2" t="s">
-        <v>665</v>
+        <v>643</v>
       </c>
       <c r="BK2" t="s">
         <v>423</v>
@@ -6815,19 +6747,19 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>666</v>
+        <v>644</v>
       </c>
       <c r="G3" t="s">
-        <v>667</v>
+        <v>645</v>
       </c>
       <c r="H3" t="s">
-        <v>668</v>
+        <v>646</v>
       </c>
       <c r="I3" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
       <c r="M3" t="s">
-        <v>670</v>
+        <v>648</v>
       </c>
       <c r="N3" t="s">
         <v>144</v>
@@ -6887,49 +6819,49 @@
         <v>443</v>
       </c>
       <c r="AO3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AP3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AQ3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AR3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AT3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AU3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AV3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AW3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AY3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="AZ3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="BA3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="BB3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="BD3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="BE3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="BF3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="BG3" t="s">
         <v>445</v>
@@ -7010,82 +6942,82 @@
         <v>251</v>
       </c>
       <c r="E1" t="s">
-        <v>572</v>
+        <v>550</v>
       </c>
       <c r="F1" t="s">
+        <v>650</v>
+      </c>
+      <c r="G1" t="s">
+        <v>651</v>
+      </c>
+      <c r="H1" t="s">
+        <v>652</v>
+      </c>
+      <c r="I1" t="s">
+        <v>653</v>
+      </c>
+      <c r="J1" t="s">
+        <v>654</v>
+      </c>
+      <c r="K1" t="s">
+        <v>655</v>
+      </c>
+      <c r="L1" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" t="s">
+        <v>658</v>
+      </c>
+      <c r="O1" t="s">
+        <v>659</v>
+      </c>
+      <c r="P1" t="s">
+        <v>660</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>661</v>
+      </c>
+      <c r="R1" t="s">
+        <v>662</v>
+      </c>
+      <c r="S1" t="s">
+        <v>663</v>
+      </c>
+      <c r="T1" t="s">
+        <v>664</v>
+      </c>
+      <c r="U1" t="s">
+        <v>665</v>
+      </c>
+      <c r="V1" t="s">
+        <v>666</v>
+      </c>
+      <c r="W1" t="s">
+        <v>667</v>
+      </c>
+      <c r="X1" t="s">
+        <v>668</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>669</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>670</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>671</v>
+      </c>
+      <c r="AB1" t="s">
         <v>672</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AC1" t="s">
         <v>673</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AD1" t="s">
         <v>674</v>
-      </c>
-      <c r="I1" t="s">
-        <v>675</v>
-      </c>
-      <c r="J1" t="s">
-        <v>676</v>
-      </c>
-      <c r="K1" t="s">
-        <v>677</v>
-      </c>
-      <c r="L1" t="s">
-        <v>678</v>
-      </c>
-      <c r="M1" t="s">
-        <v>679</v>
-      </c>
-      <c r="N1" t="s">
-        <v>680</v>
-      </c>
-      <c r="O1" t="s">
-        <v>681</v>
-      </c>
-      <c r="P1" t="s">
-        <v>682</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>683</v>
-      </c>
-      <c r="R1" t="s">
-        <v>684</v>
-      </c>
-      <c r="S1" t="s">
-        <v>685</v>
-      </c>
-      <c r="T1" t="s">
-        <v>686</v>
-      </c>
-      <c r="U1" t="s">
-        <v>687</v>
-      </c>
-      <c r="V1" t="s">
-        <v>688</v>
-      </c>
-      <c r="W1" t="s">
-        <v>689</v>
-      </c>
-      <c r="X1" t="s">
-        <v>690</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>691</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>692</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>693</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>694</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>695</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
@@ -7096,16 +7028,16 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>697</v>
+        <v>675</v>
       </c>
       <c r="D2" t="s">
-        <v>698</v>
+        <v>676</v>
       </c>
       <c r="E2" t="s">
-        <v>699</v>
+        <v>677</v>
       </c>
       <c r="F2" t="s">
-        <v>700</v>
+        <v>678</v>
       </c>
       <c r="G2" t="s">
         <v>352</v>
@@ -7120,28 +7052,28 @@
         <v>211</v>
       </c>
       <c r="K2" t="s">
-        <v>701</v>
+        <v>679</v>
       </c>
       <c r="N2" t="s">
-        <v>702</v>
+        <v>680</v>
       </c>
       <c r="O2" t="s">
-        <v>703</v>
+        <v>681</v>
       </c>
       <c r="P2" t="s">
-        <v>704</v>
+        <v>682</v>
       </c>
       <c r="Q2" t="s">
-        <v>705</v>
+        <v>683</v>
       </c>
       <c r="R2" t="s">
-        <v>706</v>
+        <v>684</v>
       </c>
       <c r="T2" t="s">
-        <v>707</v>
+        <v>685</v>
       </c>
       <c r="U2" t="s">
-        <v>708</v>
+        <v>686</v>
       </c>
       <c r="V2" t="s">
         <v>230</v>
@@ -7153,22 +7085,22 @@
         <v>232</v>
       </c>
       <c r="Y2" t="s">
-        <v>709</v>
+        <v>687</v>
       </c>
       <c r="Z2" t="s">
-        <v>710</v>
+        <v>688</v>
       </c>
       <c r="AA2" t="s">
-        <v>711</v>
+        <v>689</v>
       </c>
       <c r="AB2" t="s">
-        <v>712</v>
+        <v>690</v>
       </c>
       <c r="AC2" t="s">
-        <v>713</v>
+        <v>691</v>
       </c>
       <c r="AD2" t="s">
-        <v>714</v>
+        <v>692</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -7185,16 +7117,16 @@
         <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="L3" t="s">
-        <v>715</v>
+        <v>693</v>
       </c>
       <c r="M3" t="s">
         <v>146</v>
       </c>
       <c r="P3" t="s">
-        <v>716</v>
+        <v>694</v>
       </c>
       <c r="Q3" t="s">
         <v>150</v>
@@ -7239,136 +7171,136 @@
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B1" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D1" t="s">
+        <v>698</v>
+      </c>
+      <c r="E1" t="s">
+        <v>699</v>
+      </c>
+      <c r="F1" t="s">
+        <v>700</v>
+      </c>
+      <c r="G1" t="s">
+        <v>701</v>
+      </c>
+      <c r="H1" t="s">
+        <v>702</v>
+      </c>
+      <c r="I1" t="s">
+        <v>703</v>
+      </c>
+      <c r="J1" t="s">
+        <v>704</v>
+      </c>
+      <c r="K1" t="s">
+        <v>705</v>
+      </c>
+      <c r="L1" t="s">
+        <v>706</v>
+      </c>
+      <c r="M1" t="s">
+        <v>707</v>
+      </c>
+      <c r="N1" t="s">
+        <v>708</v>
+      </c>
+      <c r="O1" t="s">
+        <v>709</v>
+      </c>
+      <c r="P1" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>711</v>
+      </c>
+      <c r="R1" t="s">
+        <v>712</v>
+      </c>
+      <c r="S1" t="s">
+        <v>713</v>
+      </c>
+      <c r="T1" t="s">
+        <v>714</v>
+      </c>
+      <c r="U1" t="s">
+        <v>715</v>
+      </c>
+      <c r="V1" t="s">
+        <v>716</v>
+      </c>
+      <c r="W1" t="s">
         <v>717</v>
       </c>
-      <c r="B1" t="s">
+      <c r="X1" t="s">
         <v>718</v>
       </c>
-      <c r="C1" t="s">
+      <c r="Y1" t="s">
         <v>719</v>
       </c>
-      <c r="D1" t="s">
+      <c r="Z1" t="s">
         <v>720</v>
       </c>
-      <c r="E1" t="s">
+      <c r="AA1" t="s">
         <v>721</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AB1" t="s">
         <v>722</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AC1" t="s">
         <v>723</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AD1" t="s">
         <v>724</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AE1" t="s">
         <v>725</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AF1" t="s">
         <v>726</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AG1" t="s">
         <v>727</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AH1" t="s">
         <v>728</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AI1" t="s">
         <v>729</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AJ1" t="s">
         <v>730</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AK1" t="s">
         <v>731</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AL1" t="s">
         <v>732</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AM1" t="s">
         <v>733</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AN1" t="s">
         <v>734</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AO1" t="s">
         <v>735</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AP1" t="s">
         <v>736</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AQ1" t="s">
         <v>737</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AR1" t="s">
         <v>738</v>
-      </c>
-      <c r="W1" t="s">
-        <v>739</v>
-      </c>
-      <c r="X1" t="s">
-        <v>740</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>741</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>742</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>743</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>744</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>745</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>746</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>747</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>748</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>749</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>750</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>751</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>752</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>753</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>754</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>755</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>756</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>757</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>758</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>759</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
@@ -7451,783 +7383,783 @@
         <v>262</v>
       </c>
       <c r="AA2" t="s">
-        <v>761</v>
+        <v>739</v>
       </c>
       <c r="AB2" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
       <c r="AC2" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="AD2" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="AE2" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="AF2" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="AG2" t="s">
-        <v>672</v>
+        <v>650</v>
       </c>
       <c r="AH2" t="s">
-        <v>762</v>
+        <v>740</v>
       </c>
       <c r="AI2" t="s">
-        <v>678</v>
+        <v>656</v>
       </c>
       <c r="AJ2" t="s">
-        <v>680</v>
+        <v>658</v>
       </c>
       <c r="AK2" t="s">
-        <v>682</v>
+        <v>660</v>
       </c>
       <c r="AL2" t="s">
-        <v>685</v>
+        <v>663</v>
       </c>
       <c r="AM2" t="s">
-        <v>575</v>
+        <v>553</v>
       </c>
       <c r="AN2" t="s">
-        <v>579</v>
+        <v>557</v>
       </c>
       <c r="AO2" t="s">
-        <v>574</v>
+        <v>552</v>
       </c>
       <c r="AP2" t="s">
-        <v>576</v>
+        <v>554</v>
       </c>
       <c r="AQ2" t="s">
-        <v>581</v>
+        <v>559</v>
       </c>
       <c r="AR2" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
-        <v>763</v>
+        <v>741</v>
       </c>
       <c r="H3" t="s">
-        <v>764</v>
+        <v>742</v>
       </c>
       <c r="I3" t="s">
-        <v>765</v>
+        <v>743</v>
       </c>
       <c r="U3" t="s">
-        <v>764</v>
+        <v>742</v>
       </c>
       <c r="AM3" t="s">
-        <v>641</v>
+        <v>619</v>
       </c>
       <c r="AO3" t="s">
-        <v>766</v>
+        <v>744</v>
       </c>
       <c r="AP3" t="s">
-        <v>767</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>768</v>
+        <v>746</v>
       </c>
       <c r="B4" t="s">
-        <v>769</v>
+        <v>747</v>
       </c>
       <c r="C4" t="s">
-        <v>770</v>
+        <v>748</v>
       </c>
       <c r="D4" t="s">
-        <v>771</v>
+        <v>749</v>
       </c>
       <c r="E4" t="s">
         <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>772</v>
+        <v>750</v>
       </c>
       <c r="G4" t="s">
-        <v>773</v>
+        <v>751</v>
       </c>
       <c r="H4" t="s">
-        <v>774</v>
+        <v>752</v>
       </c>
       <c r="I4" t="s">
-        <v>775</v>
+        <v>753</v>
       </c>
       <c r="J4" t="s">
-        <v>776</v>
+        <v>754</v>
       </c>
       <c r="K4" t="s">
         <v>164</v>
       </c>
       <c r="L4" t="s">
+        <v>755</v>
+      </c>
+      <c r="M4" t="s">
+        <v>756</v>
+      </c>
+      <c r="N4" t="s">
+        <v>757</v>
+      </c>
+      <c r="O4" t="s">
+        <v>758</v>
+      </c>
+      <c r="P4" t="s">
+        <v>759</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>760</v>
+      </c>
+      <c r="R4" t="s">
+        <v>748</v>
+      </c>
+      <c r="S4" t="s">
+        <v>748</v>
+      </c>
+      <c r="T4" t="s">
+        <v>761</v>
+      </c>
+      <c r="U4" t="s">
+        <v>762</v>
+      </c>
+      <c r="V4" t="s">
+        <v>763</v>
+      </c>
+      <c r="W4" t="s">
+        <v>764</v>
+      </c>
+      <c r="X4" t="s">
+        <v>748</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>748</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>765</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>766</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>767</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>756</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>768</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>759</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>769</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>770</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>757</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>771</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>772</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>773</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>774</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>775</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>776</v>
+      </c>
+      <c r="AO4" t="s">
         <v>777</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AP4" t="s">
         <v>778</v>
       </c>
-      <c r="N4" t="s">
-        <v>779</v>
-      </c>
-      <c r="O4" t="s">
-        <v>780</v>
-      </c>
-      <c r="P4" t="s">
-        <v>781</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>782</v>
-      </c>
-      <c r="R4" t="s">
-        <v>770</v>
-      </c>
-      <c r="S4" t="s">
-        <v>770</v>
-      </c>
-      <c r="T4" t="s">
-        <v>783</v>
-      </c>
-      <c r="U4" t="s">
-        <v>784</v>
-      </c>
-      <c r="V4" t="s">
-        <v>785</v>
-      </c>
-      <c r="W4" t="s">
-        <v>786</v>
-      </c>
-      <c r="X4" t="s">
-        <v>770</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>770</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>787</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>788</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>789</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>778</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>790</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>781</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>791</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>792</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>779</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>793</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>794</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>795</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>796</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>797</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>798</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>799</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>800</v>
-      </c>
       <c r="AQ4" t="s">
-        <v>770</v>
+        <v>748</v>
       </c>
       <c r="AR4" t="s">
-        <v>786</v>
+        <v>764</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>779</v>
+      </c>
+      <c r="B5" t="s">
+        <v>780</v>
+      </c>
+      <c r="D5" t="s">
+        <v>781</v>
+      </c>
+      <c r="E5" t="s">
+        <v>782</v>
+      </c>
+      <c r="F5" t="s">
+        <v>783</v>
+      </c>
+      <c r="G5" t="s">
+        <v>784</v>
+      </c>
+      <c r="H5" t="s">
+        <v>785</v>
+      </c>
+      <c r="I5" t="s">
+        <v>786</v>
+      </c>
+      <c r="J5" t="s">
+        <v>787</v>
+      </c>
+      <c r="K5" t="s">
+        <v>788</v>
+      </c>
+      <c r="L5" t="s">
+        <v>789</v>
+      </c>
+      <c r="M5" t="s">
+        <v>790</v>
+      </c>
+      <c r="N5" t="s">
+        <v>791</v>
+      </c>
+      <c r="O5" t="s">
+        <v>792</v>
+      </c>
+      <c r="P5" t="s">
+        <v>793</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>794</v>
+      </c>
+      <c r="T5" t="s">
+        <v>795</v>
+      </c>
+      <c r="U5" t="s">
+        <v>796</v>
+      </c>
+      <c r="V5" t="s">
+        <v>797</v>
+      </c>
+      <c r="W5" t="s">
+        <v>798</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>799</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>800</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>790</v>
+      </c>
+      <c r="AD5" t="s">
         <v>801</v>
       </c>
-      <c r="B5" t="s">
+      <c r="AE5" t="s">
+        <v>793</v>
+      </c>
+      <c r="AF5" t="s">
         <v>802</v>
       </c>
-      <c r="D5" t="s">
+      <c r="AG5" t="s">
         <v>803</v>
       </c>
-      <c r="E5" t="s">
+      <c r="AH5" t="s">
+        <v>791</v>
+      </c>
+      <c r="AI5" t="s">
         <v>804</v>
       </c>
-      <c r="F5" t="s">
+      <c r="AJ5" t="s">
         <v>805</v>
       </c>
-      <c r="G5" t="s">
+      <c r="AK5" t="s">
         <v>806</v>
       </c>
-      <c r="H5" t="s">
+      <c r="AL5" t="s">
         <v>807</v>
       </c>
-      <c r="I5" t="s">
+      <c r="AM5" t="s">
         <v>808</v>
       </c>
-      <c r="J5" t="s">
+      <c r="AN5" t="s">
         <v>809</v>
       </c>
-      <c r="K5" t="s">
+      <c r="AO5" t="s">
         <v>810</v>
       </c>
-      <c r="L5" t="s">
+      <c r="AP5" t="s">
         <v>811</v>
       </c>
-      <c r="M5" t="s">
-        <v>812</v>
-      </c>
-      <c r="N5" t="s">
-        <v>813</v>
-      </c>
-      <c r="O5" t="s">
-        <v>814</v>
-      </c>
-      <c r="P5" t="s">
-        <v>815</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>816</v>
-      </c>
-      <c r="T5" t="s">
-        <v>817</v>
-      </c>
-      <c r="U5" t="s">
-        <v>818</v>
-      </c>
-      <c r="V5" t="s">
-        <v>819</v>
-      </c>
-      <c r="W5" t="s">
-        <v>820</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>821</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>822</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>812</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>823</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>815</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>824</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>825</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>813</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>826</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>827</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>828</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>829</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>830</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>831</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>832</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>833</v>
-      </c>
       <c r="AR5" t="s">
-        <v>820</v>
+        <v>798</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>834</v>
+        <v>812</v>
       </c>
       <c r="B6" t="s">
-        <v>835</v>
+        <v>813</v>
       </c>
       <c r="D6" t="s">
-        <v>836</v>
+        <v>814</v>
       </c>
       <c r="E6" t="s">
-        <v>837</v>
+        <v>815</v>
       </c>
       <c r="F6" t="s">
         <v>166</v>
       </c>
       <c r="G6" t="s">
-        <v>838</v>
+        <v>816</v>
       </c>
       <c r="H6" t="s">
-        <v>839</v>
+        <v>817</v>
       </c>
       <c r="I6" t="s">
-        <v>840</v>
+        <v>818</v>
       </c>
       <c r="J6" t="s">
-        <v>841</v>
+        <v>819</v>
       </c>
       <c r="L6" t="s">
-        <v>842</v>
+        <v>820</v>
       </c>
       <c r="M6" t="s">
-        <v>843</v>
+        <v>821</v>
       </c>
       <c r="N6" t="s">
-        <v>844</v>
+        <v>822</v>
       </c>
       <c r="O6" t="s">
-        <v>845</v>
+        <v>823</v>
       </c>
       <c r="P6" t="s">
-        <v>846</v>
+        <v>824</v>
       </c>
       <c r="Q6" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="T6" t="s">
-        <v>847</v>
+        <v>825</v>
       </c>
       <c r="U6" t="s">
-        <v>848</v>
+        <v>826</v>
       </c>
       <c r="V6" t="s">
-        <v>849</v>
+        <v>827</v>
       </c>
       <c r="W6" t="s">
-        <v>850</v>
+        <v>828</v>
       </c>
       <c r="AA6" t="s">
-        <v>851</v>
+        <v>829</v>
       </c>
       <c r="AB6" t="s">
-        <v>852</v>
+        <v>830</v>
       </c>
       <c r="AC6" t="s">
-        <v>843</v>
+        <v>821</v>
       </c>
       <c r="AE6" t="s">
-        <v>846</v>
+        <v>824</v>
       </c>
       <c r="AF6" t="s">
-        <v>853</v>
+        <v>831</v>
       </c>
       <c r="AG6" t="s">
-        <v>854</v>
+        <v>832</v>
       </c>
       <c r="AH6" t="s">
-        <v>855</v>
+        <v>833</v>
       </c>
       <c r="AI6" t="s">
-        <v>856</v>
+        <v>834</v>
       </c>
       <c r="AJ6" t="s">
+        <v>815</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>835</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>836</v>
+      </c>
+      <c r="AO6" t="s">
         <v>837</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>857</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>858</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>859</v>
       </c>
       <c r="AP6" t="s">
         <v>36</v>
       </c>
       <c r="AR6" t="s">
-        <v>850</v>
+        <v>828</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>860</v>
+        <v>838</v>
       </c>
       <c r="B7" t="s">
-        <v>861</v>
+        <v>839</v>
       </c>
       <c r="F7" t="s">
-        <v>862</v>
+        <v>840</v>
       </c>
       <c r="G7" t="s">
-        <v>863</v>
+        <v>841</v>
       </c>
       <c r="H7" t="s">
-        <v>864</v>
+        <v>842</v>
       </c>
       <c r="J7" t="s">
-        <v>865</v>
+        <v>843</v>
       </c>
       <c r="L7" t="s">
-        <v>866</v>
+        <v>844</v>
       </c>
       <c r="M7" t="s">
-        <v>867</v>
+        <v>845</v>
       </c>
       <c r="N7" t="s">
-        <v>868</v>
+        <v>846</v>
       </c>
       <c r="P7" t="s">
-        <v>869</v>
+        <v>847</v>
       </c>
       <c r="T7" t="s">
-        <v>870</v>
+        <v>848</v>
       </c>
       <c r="U7" t="s">
-        <v>871</v>
+        <v>849</v>
       </c>
       <c r="V7" t="s">
-        <v>872</v>
+        <v>850</v>
       </c>
       <c r="W7" t="s">
-        <v>873</v>
+        <v>851</v>
       </c>
       <c r="AC7" t="s">
-        <v>867</v>
+        <v>845</v>
       </c>
       <c r="AE7" t="s">
-        <v>869</v>
+        <v>847</v>
       </c>
       <c r="AF7" t="s">
-        <v>874</v>
+        <v>852</v>
       </c>
       <c r="AG7" t="s">
-        <v>875</v>
+        <v>853</v>
       </c>
       <c r="AI7" t="s">
-        <v>876</v>
+        <v>854</v>
       </c>
       <c r="AM7" t="s">
-        <v>877</v>
+        <v>855</v>
       </c>
       <c r="AN7" t="s">
-        <v>878</v>
+        <v>856</v>
       </c>
       <c r="AO7" t="s">
-        <v>879</v>
+        <v>857</v>
       </c>
       <c r="AP7" t="s">
-        <v>880</v>
+        <v>858</v>
       </c>
       <c r="AR7" t="s">
-        <v>873</v>
+        <v>851</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>881</v>
+        <v>859</v>
       </c>
       <c r="B8" t="s">
-        <v>882</v>
+        <v>860</v>
       </c>
       <c r="F8" t="s">
-        <v>883</v>
+        <v>861</v>
       </c>
       <c r="G8" t="s">
-        <v>884</v>
+        <v>862</v>
       </c>
       <c r="H8" t="s">
-        <v>885</v>
+        <v>863</v>
       </c>
       <c r="J8" t="s">
-        <v>886</v>
+        <v>864</v>
       </c>
       <c r="L8" t="s">
-        <v>887</v>
+        <v>865</v>
       </c>
       <c r="M8" t="s">
-        <v>888</v>
+        <v>866</v>
       </c>
       <c r="N8" t="s">
-        <v>889</v>
+        <v>867</v>
       </c>
       <c r="P8" t="s">
-        <v>890</v>
+        <v>868</v>
       </c>
       <c r="T8" t="s">
-        <v>891</v>
+        <v>869</v>
       </c>
       <c r="U8" t="s">
-        <v>892</v>
+        <v>870</v>
       </c>
       <c r="V8" t="s">
-        <v>893</v>
+        <v>871</v>
       </c>
       <c r="W8" t="s">
-        <v>837</v>
+        <v>815</v>
       </c>
       <c r="AC8" t="s">
-        <v>888</v>
+        <v>866</v>
       </c>
       <c r="AE8" t="s">
-        <v>890</v>
+        <v>868</v>
       </c>
       <c r="AG8" t="s">
-        <v>894</v>
+        <v>872</v>
       </c>
       <c r="AM8" t="s">
-        <v>895</v>
+        <v>873</v>
       </c>
       <c r="AN8" t="s">
-        <v>896</v>
+        <v>874</v>
       </c>
       <c r="AO8" t="s">
-        <v>897</v>
+        <v>875</v>
       </c>
       <c r="AP8" t="s">
-        <v>571</v>
+        <v>549</v>
       </c>
       <c r="AR8" t="s">
-        <v>837</v>
+        <v>815</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>898</v>
+        <v>876</v>
       </c>
       <c r="B9" t="s">
-        <v>899</v>
+        <v>877</v>
       </c>
       <c r="F9" t="s">
-        <v>900</v>
+        <v>878</v>
       </c>
       <c r="G9" t="s">
-        <v>901</v>
+        <v>879</v>
       </c>
       <c r="H9" t="s">
-        <v>902</v>
+        <v>880</v>
       </c>
       <c r="J9" t="s">
-        <v>903</v>
+        <v>881</v>
       </c>
       <c r="L9" t="s">
-        <v>904</v>
+        <v>882</v>
       </c>
       <c r="M9" t="s">
-        <v>905</v>
+        <v>883</v>
       </c>
       <c r="P9" t="s">
-        <v>906</v>
+        <v>884</v>
       </c>
       <c r="T9" t="s">
-        <v>907</v>
+        <v>885</v>
       </c>
       <c r="U9" t="s">
-        <v>908</v>
+        <v>886</v>
       </c>
       <c r="AE9" t="s">
-        <v>909</v>
+        <v>887</v>
       </c>
       <c r="AG9" t="s">
-        <v>905</v>
+        <v>883</v>
       </c>
       <c r="AM9" t="s">
-        <v>910</v>
+        <v>888</v>
       </c>
       <c r="AN9" t="s">
-        <v>911</v>
+        <v>889</v>
       </c>
       <c r="AO9" t="s">
-        <v>912</v>
+        <v>890</v>
       </c>
       <c r="AP9" t="s">
-        <v>913</v>
+        <v>891</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>914</v>
+        <v>892</v>
       </c>
       <c r="B10" t="s">
-        <v>915</v>
+        <v>893</v>
       </c>
       <c r="F10" t="s">
-        <v>916</v>
+        <v>894</v>
       </c>
       <c r="G10" t="s">
-        <v>917</v>
+        <v>895</v>
       </c>
       <c r="H10" t="s">
-        <v>918</v>
+        <v>896</v>
       </c>
       <c r="U10" t="s">
-        <v>919</v>
+        <v>897</v>
       </c>
       <c r="AM10" t="s">
-        <v>920</v>
+        <v>898</v>
       </c>
       <c r="AN10" t="s">
-        <v>921</v>
+        <v>899</v>
       </c>
       <c r="AO10" t="s">
-        <v>922</v>
+        <v>900</v>
       </c>
       <c r="AP10" t="s">
-        <v>923</v>
+        <v>901</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>924</v>
+        <v>902</v>
       </c>
       <c r="F11" t="s">
-        <v>925</v>
+        <v>903</v>
       </c>
       <c r="H11" t="s">
-        <v>926</v>
+        <v>904</v>
       </c>
       <c r="U11" t="s">
-        <v>927</v>
+        <v>905</v>
       </c>
       <c r="AM11" t="s">
-        <v>928</v>
+        <v>906</v>
       </c>
       <c r="AN11" t="s">
-        <v>929</v>
+        <v>907</v>
       </c>
       <c r="AO11" t="s">
-        <v>929</v>
+        <v>907</v>
       </c>
       <c r="AP11" t="s">
-        <v>930</v>
+        <v>908</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
-        <v>931</v>
+        <v>909</v>
       </c>
       <c r="U12" t="s">
-        <v>932</v>
+        <v>910</v>
       </c>
       <c r="AM12" t="s">
-        <v>933</v>
+        <v>911</v>
       </c>
       <c r="AN12" t="s">
-        <v>934</v>
+        <v>912</v>
       </c>
       <c r="AO12" t="s">
-        <v>935</v>
+        <v>913</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U13" t="s">
-        <v>936</v>
+        <v>914</v>
       </c>
       <c r="AM13" t="s">
-        <v>937</v>
+        <v>915</v>
       </c>
       <c r="AN13" t="s">
-        <v>938</v>
+        <v>916</v>
       </c>
       <c r="AO13" t="s">
-        <v>939</v>
+        <v>917</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U14" t="s">
-        <v>940</v>
+        <v>918</v>
       </c>
       <c r="AN14" t="s">
-        <v>941</v>
+        <v>919</v>
       </c>
       <c r="AO14" t="s">
-        <v>942</v>
+        <v>920</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U15" t="s">
-        <v>943</v>
+        <v>921</v>
       </c>
       <c r="AN15" t="s">
-        <v>944</v>
+        <v>922</v>
       </c>
       <c r="AO15" t="s">
-        <v>945</v>
+        <v>923</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U16" t="s">
-        <v>946</v>
+        <v>924</v>
       </c>
       <c r="AN16" t="s">
-        <v>947</v>
+        <v>925</v>
       </c>
       <c r="AO16" t="s">
-        <v>948</v>
+        <v>926</v>
       </c>
     </row>
     <row r="17" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN17" t="s">
-        <v>949</v>
+        <v>927</v>
       </c>
       <c r="AO17" t="s">
-        <v>950</v>
+        <v>928</v>
       </c>
     </row>
     <row r="18" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN18" t="s">
-        <v>951</v>
+        <v>929</v>
       </c>
       <c r="AO18" t="s">
-        <v>952</v>
+        <v>930</v>
       </c>
     </row>
     <row r="19" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN19" t="s">
-        <v>953</v>
+        <v>931</v>
       </c>
       <c r="AO19" t="s">
-        <v>954</v>
+        <v>932</v>
       </c>
     </row>
     <row r="20" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN20" t="s">
-        <v>955</v>
+        <v>933</v>
       </c>
       <c r="AO20" t="s">
-        <v>956</v>
+        <v>934</v>
       </c>
     </row>
     <row r="21" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN21" t="s">
-        <v>957</v>
+        <v>935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>